<commit_message>
Fixed assignments for Feeder 4 power quality (voltage meter). Implemented KPP5 measures Started implementation of KPP7 parameters.
</commit_message>
<xml_diff>
--- a/DistributionSystems/SimulinkOpal/Banshee/ESS_Stimuli.xlsx
+++ b/DistributionSystems/SimulinkOpal/Banshee/ESS_Stimuli.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="72" windowWidth="22980" windowHeight="9528" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="72" windowWidth="9384" windowHeight="6372" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="F4_tests" sheetId="1" r:id="rId1"/>
@@ -4455,7 +4455,7 @@
   <dimension ref="A1:AM11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AI5" sqref="AI5"/>
+      <selection activeCell="AF30" sqref="AF30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>